<commit_message>
Added formatting to graphs, ready for integration into master document
</commit_message>
<xml_diff>
--- a/CMQA/Constraint References/RCl-A-STR1 Satellite Architecture Comparison.xlsx
+++ b/CMQA/Constraint References/RCl-A-STR1 Satellite Architecture Comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Satellite Type Comparison" sheetId="4" r:id="rId1"/>
@@ -170,6 +170,32 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Microsatellites and CubeSats Per Launch: 2010-2013</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -796,6 +822,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="107308160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -815,6 +854,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="107298176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -824,6 +876,19 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -846,6 +911,39 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>University Microsatellites and</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> CubeSats Per Launch: 2010-2013</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1282,6 +1380,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="101017856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1301,6 +1412,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="101016320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1310,6 +1434,19 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1332,6 +1469,39 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Launced Microsatellties</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> and CubeSats: 2010-2013</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1440,6 +1610,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="107886464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1449,6 +1632,19 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1471,6 +1667,39 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Launched University Nanosatellites</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> and CubeSats: 2010-2013</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1579,6 +1808,19 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="109049728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1588,6 +1830,19 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1622,7 +1877,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1633,7 +1888,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added pie chart comparisons
</commit_message>
<xml_diff>
--- a/CMQA/Constraint References/RCl-A-STR1 Satellite Architecture Comparison.xlsx
+++ b/CMQA/Constraint References/RCl-A-STR1 Satellite Architecture Comparison.xlsx
@@ -4,23 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="24915" windowHeight="12015" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Satellite Type Comparison" sheetId="4" r:id="rId1"/>
     <sheet name="University Sat Comparison" sheetId="5" r:id="rId2"/>
     <sheet name="Total Comparison" sheetId="6" r:id="rId3"/>
     <sheet name="Total University Comparison" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
+    <sheet name="Total Smallsat Pie Chart" sheetId="8" r:id="rId5"/>
+    <sheet name="University Sat Pie Chart" sheetId="9" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId8"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Launch Name</t>
   </si>
@@ -105,11 +107,26 @@
   <si>
     <t>Total</t>
   </si>
+  <si>
+    <t>Total CubeSat Percentage</t>
+  </si>
+  <si>
+    <t>Total MicroSat Percentage</t>
+  </si>
+  <si>
+    <t>University CubeSat Percentage</t>
+  </si>
+  <si>
+    <t>University MircoSat Percentage</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,9 +156,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1851,6 +1870,256 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Total</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> Microsatellite vs. Total CubeSat Comparison: 2010-2013</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$34:$E$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Total CubeSat Percentage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total MicroSat Percentage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$34:$F$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>70.224719101123597</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.775280898876407</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>University Microsatelltie</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> vs. University CubeSat Comparison: 2010-2013</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1600">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$38:$E$39</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>University CubeSat Percentage</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>University MircoSat Percentage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$38:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>80.434782608695656</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.565217391304348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -1888,7 +2157,29 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1977,6 +2268,60 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8674835" cy="6297521"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8674835" cy="6297521"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
@@ -2290,17 +2635,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I32"/>
+  <dimension ref="C2:I40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" activeCellId="2" sqref="E32 H32 I32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
@@ -3020,6 +3365,56 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
+    </row>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="3">
+        <f>F32/H34*100</f>
+        <v>70.224719101123597</v>
+      </c>
+      <c r="H34">
+        <f>SUM(F32:G32)</f>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="3">
+        <f>G32/H34*100</f>
+        <v>29.775280898876407</v>
+      </c>
+      <c r="H35">
+        <f>SUM(H32:I32)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="3">
+        <f>H32/H35*100</f>
+        <v>80.434782608695656</v>
+      </c>
+    </row>
+    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="2">
+        <f>I32/H35*100</f>
+        <v>19.565217391304348</v>
+      </c>
+    </row>
+    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>